<commit_message>
Update files for Project
</commit_message>
<xml_diff>
--- a/data/raw/03 Corpus Semiologia.xlsx
+++ b/data/raw/03 Corpus Semiologia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\FERNANDOHC\EDUCACION\MAESTRIA\UNI_MAI\SEMESTRE_4\MIA-403 Proyecto de investigación II\Repositorio\MIA403-TraductorQuechuaEspaniol\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2281ABEA-5BFE-42E0-BCD0-40FFC5C84A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A490B6D-4C97-4343-950D-8A04BC93FC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,13 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="619">
-  <si>
-    <t>ESPAÑOL</t>
-  </si>
-  <si>
-    <t>QUECHUA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="617">
   <si>
     <t>Buenas noches, señor / señora / joven / señorita</t>
   </si>
@@ -2202,15 +2196,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B311"/>
+  <dimension ref="A1:B310"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.5546875" customWidth="1"/>
+    <col min="1" max="1" width="68.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -2506,15 +2500,15 @@
         <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" t="s">
         <v>74</v>
-      </c>
-      <c r="B38" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -2538,15 +2532,15 @@
         <v>79</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" t="s">
         <v>81</v>
-      </c>
-      <c r="B42" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -3999,15 +3993,15 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
+        <v>364</v>
+      </c>
+      <c r="B224" t="s">
         <v>444</v>
-      </c>
-      <c r="B224" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>366</v>
+        <v>445</v>
       </c>
       <c r="B225" t="s">
         <v>446</v>
@@ -4691,14 +4685,6 @@
       </c>
       <c r="B310" t="s">
         <v>616</v>
-      </c>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A311" t="s">
-        <v>617</v>
-      </c>
-      <c r="B311" t="s">
-        <v>618</v>
       </c>
     </row>
   </sheetData>

</xml_diff>